<commit_message>
creación de pegado desde excel
</commit_message>
<xml_diff>
--- a/project-root/uploads/alumnos1.xlsx
+++ b/project-root/uploads/alumnos1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df88bd836257aa85/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0F8573C-609A-46EA-A4D8-0C4D957725DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{E0F8573C-609A-46EA-A4D8-0C4D957725DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B37B403B-20A4-42B3-88F5-89438C718073}"/>
   <bookViews>
     <workbookView xWindow="2820" yWindow="2352" windowWidth="12564" windowHeight="9372" xr2:uid="{F55863C4-0B39-4EE9-9BE5-DE3081128254}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>nombre</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>21M016</t>
+  </si>
+  <si>
+    <t>curso</t>
   </si>
 </sst>
 </file>
@@ -146,8 +149,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -163,6 +167,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -482,15 +490,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564AF95D-4671-4917-A9AF-37CE85342C1C}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -506,8 +514,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -523,8 +534,11 @@
       <c r="E2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -540,8 +554,11 @@
       <c r="E3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -549,7 +566,7 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -557,8 +574,11 @@
       <c r="E4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -574,8 +594,11 @@
       <c r="E5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -591,8 +614,11 @@
       <c r="E6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -608,6 +634,12 @@
       <c r="E7" t="s">
         <v>24</v>
       </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>